<commit_message>
chore: update Excel template formatting
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -69,7 +69,7 @@
     <t>비 고</t>
   </si>
   <si>
-    <t>투입인원수 산정기준</t>
+    <t>투입인원 및 내역</t>
   </si>
   <si>
     <t>업 무 구 분</t>
@@ -216,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -241,6 +241,12 @@
       <sz val="25.0"/>
       <color rgb="FF000000"/>
       <name val="HY헤드라인M"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic"/>
     </font>
     <font>
       <b/>
@@ -517,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -602,7 +608,7 @@
     <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -614,7 +620,7 @@
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="25" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="25" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -623,67 +629,70 @@
     <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="28" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="28" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="30" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="25" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="30" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1234,7 +1243,7 @@
       <c r="M19" s="18"/>
       <c r="N19" s="19"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" ht="22.5" customHeight="1">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -1269,7 +1278,7 @@
       <c r="M21" s="18"/>
       <c r="N21" s="19"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" ht="24.0" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -4549,7 +4558,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="40.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="33"/>
@@ -4587,7 +4596,7 @@
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="46"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -4597,7 +4606,7 @@
       <c r="H3" s="41"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="46"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
       <c r="D4" s="40"/>
@@ -4607,7 +4616,7 @@
       <c r="H4" s="41"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="46"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
       <c r="D5" s="40"/>
@@ -4617,7 +4626,7 @@
       <c r="H5" s="41"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="46"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -4627,7 +4636,7 @@
       <c r="H6" s="41"/>
     </row>
     <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="46"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -4637,7 +4646,7 @@
       <c r="H7" s="41"/>
     </row>
     <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="46"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
       <c r="D8" s="40"/>
@@ -4647,7 +4656,7 @@
       <c r="H8" s="41"/>
     </row>
     <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="46"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -4657,7 +4666,7 @@
       <c r="H9" s="41"/>
     </row>
     <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="46"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
@@ -4667,7 +4676,7 @@
       <c r="H10" s="41"/>
     </row>
     <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="46"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
@@ -4677,7 +4686,7 @@
       <c r="H11" s="41"/>
     </row>
     <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="46"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
@@ -4687,7 +4696,7 @@
       <c r="H12" s="41"/>
     </row>
     <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="46"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
@@ -4697,7 +4706,7 @@
       <c r="H13" s="41"/>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="46"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
@@ -4707,7 +4716,7 @@
       <c r="H14" s="41"/>
     </row>
     <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="46"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
@@ -4717,7 +4726,7 @@
       <c r="H15" s="41"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="46"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -4727,7 +4736,7 @@
       <c r="H16" s="41"/>
     </row>
     <row r="17" ht="18.75" customHeight="1">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
@@ -4737,7 +4746,7 @@
       <c r="H17" s="41"/>
     </row>
     <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="46"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
@@ -4747,7 +4756,7 @@
       <c r="H18" s="41"/>
     </row>
     <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="46"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
@@ -4757,7 +4766,7 @@
       <c r="H19" s="41"/>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="46"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="40"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
@@ -4767,7 +4776,7 @@
       <c r="H20" s="41"/>
     </row>
     <row r="21" ht="18.75" customHeight="1">
-      <c r="A21" s="46"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
@@ -4777,7 +4786,7 @@
       <c r="H21" s="41"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="46"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
@@ -4787,7 +4796,7 @@
       <c r="H22" s="41"/>
     </row>
     <row r="23" ht="18.75" customHeight="1">
-      <c r="A23" s="46"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="40"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
@@ -4797,7 +4806,7 @@
       <c r="H23" s="41"/>
     </row>
     <row r="24" ht="18.75" customHeight="1">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="40"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
@@ -4807,7 +4816,7 @@
       <c r="H24" s="41"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
-      <c r="A25" s="46"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="40"/>
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
@@ -4817,7 +4826,7 @@
       <c r="H25" s="41"/>
     </row>
     <row r="26" ht="18.75" customHeight="1">
-      <c r="A26" s="46"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
       <c r="D26" s="40"/>
@@ -4827,7 +4836,7 @@
       <c r="H26" s="41"/>
     </row>
     <row r="27" ht="18.75" customHeight="1">
-      <c r="A27" s="46"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
@@ -4837,7 +4846,7 @@
       <c r="H27" s="41"/>
     </row>
     <row r="28" ht="18.75" customHeight="1">
-      <c r="A28" s="46"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
@@ -4847,7 +4856,7 @@
       <c r="H28" s="41"/>
     </row>
     <row r="29" ht="18.75" customHeight="1">
-      <c r="A29" s="46"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="40"/>
       <c r="C29" s="40"/>
       <c r="D29" s="40"/>
@@ -4857,7 +4866,7 @@
       <c r="H29" s="41"/>
     </row>
     <row r="30" ht="18.75" customHeight="1">
-      <c r="A30" s="47"/>
+      <c r="A30" s="48"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
       <c r="D30" s="44"/>
@@ -5932,628 +5941,628 @@
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="46"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="50"/>
     </row>
     <row r="4" ht="20.25" customHeight="1">
-      <c r="A4" s="46"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="50"/>
     </row>
     <row r="5" ht="20.25" customHeight="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="50"/>
     </row>
     <row r="6" ht="20.25" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="50"/>
     </row>
     <row r="7" ht="20.25" customHeight="1">
-      <c r="A7" s="46"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" ht="20.25" customHeight="1">
-      <c r="A8" s="46"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="50"/>
     </row>
     <row r="9" ht="20.25" customHeight="1">
-      <c r="A9" s="46"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="50"/>
     </row>
     <row r="10" ht="20.25" customHeight="1">
-      <c r="A10" s="46"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="50"/>
     </row>
     <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="46"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="50"/>
     </row>
     <row r="12" ht="20.25" customHeight="1">
-      <c r="A12" s="46"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" ht="20.25" customHeight="1">
-      <c r="A13" s="46"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="50"/>
     </row>
     <row r="14" ht="20.25" customHeight="1">
-      <c r="A14" s="46"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
+      <c r="A14" s="47"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="50"/>
     </row>
     <row r="15" ht="20.25" customHeight="1">
-      <c r="A15" s="46"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="50"/>
     </row>
     <row r="16" ht="20.25" customHeight="1">
-      <c r="A16" s="46"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="50"/>
     </row>
     <row r="17" ht="20.25" customHeight="1">
-      <c r="A17" s="46"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="50"/>
     </row>
     <row r="18" ht="20.25" customHeight="1">
-      <c r="A18" s="46"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="50"/>
     </row>
     <row r="19" ht="20.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="50"/>
     </row>
     <row r="20" ht="20.25" customHeight="1">
-      <c r="A20" s="46"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="50"/>
     </row>
     <row r="21" ht="20.25" customHeight="1">
-      <c r="A21" s="46"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="50"/>
     </row>
     <row r="22" ht="20.25" customHeight="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
     </row>
     <row r="23" ht="20.25" customHeight="1">
-      <c r="A23" s="46"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50"/>
     </row>
     <row r="24" ht="20.25" customHeight="1">
-      <c r="A24" s="46"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="50"/>
     </row>
     <row r="25" ht="20.25" customHeight="1">
-      <c r="A25" s="46"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="39"/>
       <c r="I25" s="39"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="50"/>
     </row>
     <row r="26" ht="20.25" customHeight="1">
-      <c r="A26" s="46"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="50"/>
     </row>
     <row r="27" ht="20.25" customHeight="1">
-      <c r="A27" s="46"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
       <c r="H27" s="39"/>
       <c r="I27" s="39"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
     </row>
     <row r="28" ht="20.25" customHeight="1">
-      <c r="A28" s="46"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
+      <c r="A28" s="47"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
       <c r="H28" s="39"/>
       <c r="I28" s="39"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
     </row>
     <row r="29" ht="20.25" customHeight="1">
-      <c r="A29" s="46"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
+      <c r="A29" s="47"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
       <c r="H29" s="39"/>
       <c r="I29" s="39"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="50"/>
     </row>
     <row r="30" ht="20.25" customHeight="1">
-      <c r="A30" s="46"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
       <c r="H30" s="39"/>
       <c r="I30" s="39"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="50"/>
     </row>
     <row r="31" ht="20.25" customHeight="1">
-      <c r="A31" s="46"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="50"/>
     </row>
     <row r="32" ht="20.25" customHeight="1">
-      <c r="A32" s="46"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
       <c r="H32" s="39"/>
       <c r="I32" s="39"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="50"/>
     </row>
     <row r="33" ht="20.25" customHeight="1">
-      <c r="A33" s="46"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
       <c r="H33" s="39"/>
       <c r="I33" s="39"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="50"/>
     </row>
     <row r="34" ht="20.25" customHeight="1">
-      <c r="A34" s="46"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
       <c r="H34" s="39"/>
       <c r="I34" s="39"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="50"/>
     </row>
     <row r="35" ht="20.25" customHeight="1">
-      <c r="A35" s="46"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
       <c r="H35" s="39"/>
       <c r="I35" s="39"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
     </row>
     <row r="36" ht="20.25" customHeight="1">
-      <c r="A36" s="46"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
       <c r="H36" s="39"/>
       <c r="I36" s="39"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="50"/>
     </row>
     <row r="37" ht="20.25" customHeight="1">
-      <c r="A37" s="46"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
       <c r="H37" s="39"/>
       <c r="I37" s="39"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="50"/>
     </row>
     <row r="38" ht="20.25" customHeight="1">
-      <c r="A38" s="46"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
       <c r="H38" s="39"/>
       <c r="I38" s="39"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="50"/>
     </row>
     <row r="39" ht="20.25" customHeight="1">
-      <c r="A39" s="46"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
       <c r="H39" s="39"/>
       <c r="I39" s="39"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="50"/>
     </row>
     <row r="40" ht="20.25" customHeight="1">
-      <c r="A40" s="46"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
       <c r="H40" s="39"/>
       <c r="I40" s="39"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="48"/>
-      <c r="N40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="50"/>
     </row>
     <row r="41" ht="20.25" customHeight="1">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
       <c r="H41" s="43"/>
       <c r="I41" s="43"/>
-      <c r="J41" s="50"/>
-      <c r="K41" s="50"/>
-      <c r="L41" s="50"/>
-      <c r="M41" s="50"/>
-      <c r="N41" s="51"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="52"/>
     </row>
     <row r="42" ht="20.25" customHeight="1">
       <c r="H42" s="39"/>
@@ -9236,37 +9245,37 @@
       <c r="A2" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="53" t="s">
+      <c r="L2" s="54" t="s">
         <v>55</v>
       </c>
     </row>
@@ -9282,7 +9291,7 @@
       <c r="I3" s="40"/>
       <c r="J3" s="40"/>
       <c r="K3" s="40"/>
-      <c r="L3" s="54"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="38"/>
@@ -9296,7 +9305,7 @@
       <c r="I4" s="40"/>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
-      <c r="L4" s="54"/>
+      <c r="L4" s="55"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="38"/>
@@ -9310,7 +9319,7 @@
       <c r="I5" s="40"/>
       <c r="J5" s="40"/>
       <c r="K5" s="40"/>
-      <c r="L5" s="54"/>
+      <c r="L5" s="55"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
       <c r="A6" s="38"/>
@@ -9324,7 +9333,7 @@
       <c r="I6" s="40"/>
       <c r="J6" s="40"/>
       <c r="K6" s="40"/>
-      <c r="L6" s="54"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="38"/>
@@ -9338,7 +9347,7 @@
       <c r="I7" s="40"/>
       <c r="J7" s="40"/>
       <c r="K7" s="40"/>
-      <c r="L7" s="54"/>
+      <c r="L7" s="55"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="38"/>
@@ -9352,7 +9361,7 @@
       <c r="I8" s="40"/>
       <c r="J8" s="40"/>
       <c r="K8" s="40"/>
-      <c r="L8" s="54"/>
+      <c r="L8" s="55"/>
     </row>
     <row r="9" ht="21.75" customHeight="1">
       <c r="A9" s="38"/>
@@ -9366,7 +9375,7 @@
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
       <c r="K9" s="40"/>
-      <c r="L9" s="54"/>
+      <c r="L9" s="55"/>
     </row>
     <row r="10" ht="21.75" customHeight="1">
       <c r="A10" s="38"/>
@@ -9380,7 +9389,7 @@
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="40"/>
-      <c r="L10" s="54"/>
+      <c r="L10" s="55"/>
     </row>
     <row r="11" ht="21.75" customHeight="1">
       <c r="A11" s="38"/>
@@ -9394,7 +9403,7 @@
       <c r="I11" s="40"/>
       <c r="J11" s="40"/>
       <c r="K11" s="40"/>
-      <c r="L11" s="54"/>
+      <c r="L11" s="55"/>
     </row>
     <row r="12" ht="21.75" customHeight="1">
       <c r="A12" s="38"/>
@@ -9408,7 +9417,7 @@
       <c r="I12" s="40"/>
       <c r="J12" s="40"/>
       <c r="K12" s="40"/>
-      <c r="L12" s="54"/>
+      <c r="L12" s="55"/>
     </row>
     <row r="13" ht="21.75" customHeight="1">
       <c r="A13" s="38"/>
@@ -9422,7 +9431,7 @@
       <c r="I13" s="40"/>
       <c r="J13" s="40"/>
       <c r="K13" s="40"/>
-      <c r="L13" s="54"/>
+      <c r="L13" s="55"/>
     </row>
     <row r="14" ht="21.75" customHeight="1">
       <c r="A14" s="38"/>
@@ -9436,7 +9445,7 @@
       <c r="I14" s="40"/>
       <c r="J14" s="40"/>
       <c r="K14" s="40"/>
-      <c r="L14" s="54"/>
+      <c r="L14" s="55"/>
     </row>
     <row r="15" ht="21.75" customHeight="1">
       <c r="A15" s="38"/>
@@ -9450,7 +9459,7 @@
       <c r="I15" s="40"/>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
-      <c r="L15" s="54"/>
+      <c r="L15" s="55"/>
     </row>
     <row r="16" ht="21.75" customHeight="1">
       <c r="A16" s="38"/>
@@ -9464,7 +9473,7 @@
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
-      <c r="L16" s="54"/>
+      <c r="L16" s="55"/>
     </row>
     <row r="17" ht="21.75" customHeight="1">
       <c r="A17" s="38"/>
@@ -9478,7 +9487,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="54"/>
+      <c r="L17" s="55"/>
     </row>
     <row r="18" ht="21.75" customHeight="1">
       <c r="A18" s="38"/>
@@ -9492,7 +9501,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="54"/>
+      <c r="L18" s="55"/>
     </row>
     <row r="19" ht="21.75" customHeight="1">
       <c r="A19" s="38"/>
@@ -9506,7 +9515,7 @@
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
-      <c r="L19" s="54"/>
+      <c r="L19" s="55"/>
     </row>
     <row r="20" ht="21.75" customHeight="1">
       <c r="A20" s="38"/>
@@ -9520,7 +9529,7 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
       <c r="K20" s="40"/>
-      <c r="L20" s="54"/>
+      <c r="L20" s="55"/>
     </row>
     <row r="21" ht="21.75" customHeight="1">
       <c r="A21" s="38"/>
@@ -9534,7 +9543,7 @@
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
       <c r="K21" s="40"/>
-      <c r="L21" s="54"/>
+      <c r="L21" s="55"/>
     </row>
     <row r="22" ht="21.75" customHeight="1">
       <c r="A22" s="38"/>
@@ -9548,7 +9557,7 @@
       <c r="I22" s="40"/>
       <c r="J22" s="40"/>
       <c r="K22" s="40"/>
-      <c r="L22" s="54"/>
+      <c r="L22" s="55"/>
     </row>
     <row r="23" ht="21.75" customHeight="1">
       <c r="A23" s="38"/>
@@ -9562,7 +9571,7 @@
       <c r="I23" s="40"/>
       <c r="J23" s="40"/>
       <c r="K23" s="40"/>
-      <c r="L23" s="54"/>
+      <c r="L23" s="55"/>
     </row>
     <row r="24" ht="21.75" customHeight="1">
       <c r="A24" s="42"/>
@@ -9576,7 +9585,7 @@
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
-      <c r="L24" s="55"/>
+      <c r="L24" s="56"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat: update Excel template formatting
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -523,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -661,9 +661,6 @@
     </xf>
     <xf borderId="15" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf borderId="25" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
@@ -2371,7 +2368,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="2" width="21.71"/>
+    <col customWidth="1" min="2" max="2" width="28.14"/>
     <col customWidth="1" min="3" max="8" width="16.0"/>
   </cols>
   <sheetData>
@@ -4558,7 +4555,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="40.5" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="32" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="33"/>
@@ -4596,7 +4593,7 @@
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="47"/>
+      <c r="A3" s="46"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -4606,7 +4603,7 @@
       <c r="H3" s="41"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="47"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
       <c r="D4" s="40"/>
@@ -4616,7 +4613,7 @@
       <c r="H4" s="41"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="47"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
       <c r="D5" s="40"/>
@@ -4626,7 +4623,7 @@
       <c r="H5" s="41"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="47"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="40"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -4636,7 +4633,7 @@
       <c r="H6" s="41"/>
     </row>
     <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="47"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="40"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -4646,7 +4643,7 @@
       <c r="H7" s="41"/>
     </row>
     <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" s="47"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="40"/>
       <c r="C8" s="40"/>
       <c r="D8" s="40"/>
@@ -4656,7 +4653,7 @@
       <c r="H8" s="41"/>
     </row>
     <row r="9" ht="18.75" customHeight="1">
-      <c r="A9" s="47"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -4666,7 +4663,7 @@
       <c r="H9" s="41"/>
     </row>
     <row r="10" ht="18.75" customHeight="1">
-      <c r="A10" s="47"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
@@ -4676,7 +4673,7 @@
       <c r="H10" s="41"/>
     </row>
     <row r="11" ht="18.75" customHeight="1">
-      <c r="A11" s="47"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
@@ -4686,7 +4683,7 @@
       <c r="H11" s="41"/>
     </row>
     <row r="12" ht="18.75" customHeight="1">
-      <c r="A12" s="47"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
@@ -4696,7 +4693,7 @@
       <c r="H12" s="41"/>
     </row>
     <row r="13" ht="18.75" customHeight="1">
-      <c r="A13" s="47"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
@@ -4706,7 +4703,7 @@
       <c r="H13" s="41"/>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="47"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
@@ -4716,7 +4713,7 @@
       <c r="H14" s="41"/>
     </row>
     <row r="15" ht="18.75" customHeight="1">
-      <c r="A15" s="47"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="40"/>
       <c r="C15" s="40"/>
       <c r="D15" s="40"/>
@@ -4726,7 +4723,7 @@
       <c r="H15" s="41"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="47"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -4736,7 +4733,7 @@
       <c r="H16" s="41"/>
     </row>
     <row r="17" ht="18.75" customHeight="1">
-      <c r="A17" s="47"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
@@ -4746,7 +4743,7 @@
       <c r="H17" s="41"/>
     </row>
     <row r="18" ht="18.75" customHeight="1">
-      <c r="A18" s="47"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
@@ -4756,7 +4753,7 @@
       <c r="H18" s="41"/>
     </row>
     <row r="19" ht="18.75" customHeight="1">
-      <c r="A19" s="47"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
@@ -4766,7 +4763,7 @@
       <c r="H19" s="41"/>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="A20" s="47"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="40"/>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
@@ -4776,7 +4773,7 @@
       <c r="H20" s="41"/>
     </row>
     <row r="21" ht="18.75" customHeight="1">
-      <c r="A21" s="47"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
@@ -4786,7 +4783,7 @@
       <c r="H21" s="41"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="A22" s="47"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
@@ -4796,7 +4793,7 @@
       <c r="H22" s="41"/>
     </row>
     <row r="23" ht="18.75" customHeight="1">
-      <c r="A23" s="47"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="40"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
@@ -4806,7 +4803,7 @@
       <c r="H23" s="41"/>
     </row>
     <row r="24" ht="18.75" customHeight="1">
-      <c r="A24" s="47"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="40"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
@@ -4816,7 +4813,7 @@
       <c r="H24" s="41"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
-      <c r="A25" s="47"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="40"/>
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
@@ -4826,7 +4823,7 @@
       <c r="H25" s="41"/>
     </row>
     <row r="26" ht="18.75" customHeight="1">
-      <c r="A26" s="47"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
       <c r="D26" s="40"/>
@@ -4836,7 +4833,7 @@
       <c r="H26" s="41"/>
     </row>
     <row r="27" ht="18.75" customHeight="1">
-      <c r="A27" s="47"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
@@ -4846,7 +4843,7 @@
       <c r="H27" s="41"/>
     </row>
     <row r="28" ht="18.75" customHeight="1">
-      <c r="A28" s="47"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
@@ -4856,7 +4853,7 @@
       <c r="H28" s="41"/>
     </row>
     <row r="29" ht="18.75" customHeight="1">
-      <c r="A29" s="47"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="40"/>
       <c r="C29" s="40"/>
       <c r="D29" s="40"/>
@@ -4866,16 +4863,25 @@
       <c r="H29" s="41"/>
     </row>
     <row r="30" ht="18.75" customHeight="1">
-      <c r="A30" s="48"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="45"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="41"/>
+    </row>
+    <row r="31" ht="18.75" customHeight="1">
+      <c r="A31" s="47"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="45"/>
+    </row>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
@@ -5853,7 +5859,7 @@
   <pageMargins bottom="0.9843055605888367" footer="0.0" header="0.0" left="0.7480555772781372" right="0.7480555772781372" top="0.9843055605888367"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="30" man="1"/>
+    <brk id="31" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" man="1"/>
@@ -5941,638 +5947,650 @@
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="47"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="50"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" ht="20.25" customHeight="1">
-      <c r="A4" s="47"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="49"/>
     </row>
     <row r="5" ht="20.25" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="39"/>
       <c r="I5" s="39"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="50"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="49"/>
     </row>
     <row r="6" ht="20.25" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="50"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="49"/>
     </row>
     <row r="7" ht="20.25" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="50"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="49"/>
     </row>
     <row r="8" ht="20.25" customHeight="1">
-      <c r="A8" s="47"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="50"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="49"/>
     </row>
     <row r="9" ht="20.25" customHeight="1">
-      <c r="A9" s="47"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="50"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="49"/>
     </row>
     <row r="10" ht="20.25" customHeight="1">
-      <c r="A10" s="47"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="50"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="49"/>
     </row>
     <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="47"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="49"/>
     </row>
     <row r="12" ht="20.25" customHeight="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="50"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="49"/>
     </row>
     <row r="13" ht="20.25" customHeight="1">
-      <c r="A13" s="47"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="50"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="49"/>
     </row>
     <row r="14" ht="20.25" customHeight="1">
-      <c r="A14" s="47"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="50"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="49"/>
     </row>
     <row r="15" ht="20.25" customHeight="1">
-      <c r="A15" s="47"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="50"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="49"/>
     </row>
     <row r="16" ht="20.25" customHeight="1">
-      <c r="A16" s="47"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="50"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="49"/>
     </row>
     <row r="17" ht="20.25" customHeight="1">
-      <c r="A17" s="47"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="50"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="49"/>
     </row>
     <row r="18" ht="20.25" customHeight="1">
-      <c r="A18" s="47"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="50"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
     </row>
     <row r="19" ht="20.25" customHeight="1">
-      <c r="A19" s="47"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="50"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="49"/>
     </row>
     <row r="20" ht="20.25" customHeight="1">
-      <c r="A20" s="47"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="50"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="49"/>
     </row>
     <row r="21" ht="20.25" customHeight="1">
-      <c r="A21" s="47"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="50"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="49"/>
     </row>
     <row r="22" ht="20.25" customHeight="1">
-      <c r="A22" s="47"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="49"/>
     </row>
     <row r="23" ht="20.25" customHeight="1">
-      <c r="A23" s="47"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="50"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="49"/>
     </row>
     <row r="24" ht="20.25" customHeight="1">
-      <c r="A24" s="47"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="50"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="49"/>
     </row>
     <row r="25" ht="20.25" customHeight="1">
-      <c r="A25" s="47"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
       <c r="H25" s="39"/>
       <c r="I25" s="39"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="50"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="49"/>
     </row>
     <row r="26" ht="20.25" customHeight="1">
-      <c r="A26" s="47"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="50"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="49"/>
     </row>
     <row r="27" ht="20.25" customHeight="1">
-      <c r="A27" s="47"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
       <c r="H27" s="39"/>
       <c r="I27" s="39"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="50"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="49"/>
     </row>
     <row r="28" ht="20.25" customHeight="1">
-      <c r="A28" s="47"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
       <c r="H28" s="39"/>
       <c r="I28" s="39"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="50"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="49"/>
     </row>
     <row r="29" ht="20.25" customHeight="1">
-      <c r="A29" s="47"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
       <c r="H29" s="39"/>
       <c r="I29" s="39"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="50"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="49"/>
     </row>
     <row r="30" ht="20.25" customHeight="1">
-      <c r="A30" s="47"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
       <c r="H30" s="39"/>
       <c r="I30" s="39"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="50"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="49"/>
     </row>
     <row r="31" ht="20.25" customHeight="1">
-      <c r="A31" s="47"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="50"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="49"/>
     </row>
     <row r="32" ht="20.25" customHeight="1">
-      <c r="A32" s="47"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
       <c r="H32" s="39"/>
       <c r="I32" s="39"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="50"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="49"/>
     </row>
     <row r="33" ht="20.25" customHeight="1">
-      <c r="A33" s="47"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
       <c r="H33" s="39"/>
       <c r="I33" s="39"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="50"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="49"/>
     </row>
     <row r="34" ht="20.25" customHeight="1">
-      <c r="A34" s="47"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
       <c r="H34" s="39"/>
       <c r="I34" s="39"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="50"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="49"/>
     </row>
     <row r="35" ht="20.25" customHeight="1">
-      <c r="A35" s="47"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
+      <c r="A35" s="46"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
       <c r="H35" s="39"/>
       <c r="I35" s="39"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="50"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="49"/>
     </row>
     <row r="36" ht="20.25" customHeight="1">
-      <c r="A36" s="47"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
+      <c r="A36" s="46"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
       <c r="H36" s="39"/>
       <c r="I36" s="39"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="50"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="L36" s="48"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="49"/>
     </row>
     <row r="37" ht="20.25" customHeight="1">
-      <c r="A37" s="47"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
+      <c r="A37" s="46"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
       <c r="H37" s="39"/>
       <c r="I37" s="39"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="50"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="49"/>
     </row>
     <row r="38" ht="20.25" customHeight="1">
-      <c r="A38" s="47"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
       <c r="H38" s="39"/>
       <c r="I38" s="39"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="50"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="48"/>
+      <c r="N38" s="49"/>
     </row>
     <row r="39" ht="20.25" customHeight="1">
-      <c r="A39" s="47"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
       <c r="H39" s="39"/>
       <c r="I39" s="39"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="50"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="49"/>
     </row>
     <row r="40" ht="20.25" customHeight="1">
-      <c r="A40" s="47"/>
-      <c r="B40" s="49"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
       <c r="H40" s="39"/>
       <c r="I40" s="39"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="50"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="49"/>
     </row>
     <row r="41" ht="20.25" customHeight="1">
-      <c r="A41" s="48"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="52"/>
+      <c r="A41" s="46"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="49"/>
     </row>
     <row r="42" ht="20.25" customHeight="1">
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="50"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="51"/>
     </row>
     <row r="43" ht="20.25" customHeight="1">
       <c r="H43" s="39"/>
       <c r="I43" s="39"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" ht="20.25" customHeight="1">
       <c r="H44" s="39"/>
       <c r="I44" s="39"/>
     </row>
@@ -9245,37 +9263,37 @@
       <c r="A2" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="53" t="s">
+      <c r="K2" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="54" t="s">
+      <c r="L2" s="53" t="s">
         <v>55</v>
       </c>
     </row>
@@ -9291,7 +9309,7 @@
       <c r="I3" s="40"/>
       <c r="J3" s="40"/>
       <c r="K3" s="40"/>
-      <c r="L3" s="55"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" ht="21.75" customHeight="1">
       <c r="A4" s="38"/>
@@ -9305,7 +9323,7 @@
       <c r="I4" s="40"/>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
-      <c r="L4" s="55"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" ht="21.75" customHeight="1">
       <c r="A5" s="38"/>
@@ -9319,7 +9337,7 @@
       <c r="I5" s="40"/>
       <c r="J5" s="40"/>
       <c r="K5" s="40"/>
-      <c r="L5" s="55"/>
+      <c r="L5" s="54"/>
     </row>
     <row r="6" ht="21.75" customHeight="1">
       <c r="A6" s="38"/>
@@ -9333,7 +9351,7 @@
       <c r="I6" s="40"/>
       <c r="J6" s="40"/>
       <c r="K6" s="40"/>
-      <c r="L6" s="55"/>
+      <c r="L6" s="54"/>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="38"/>
@@ -9347,7 +9365,7 @@
       <c r="I7" s="40"/>
       <c r="J7" s="40"/>
       <c r="K7" s="40"/>
-      <c r="L7" s="55"/>
+      <c r="L7" s="54"/>
     </row>
     <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="38"/>
@@ -9361,7 +9379,7 @@
       <c r="I8" s="40"/>
       <c r="J8" s="40"/>
       <c r="K8" s="40"/>
-      <c r="L8" s="55"/>
+      <c r="L8" s="54"/>
     </row>
     <row r="9" ht="21.75" customHeight="1">
       <c r="A9" s="38"/>
@@ -9375,7 +9393,7 @@
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
       <c r="K9" s="40"/>
-      <c r="L9" s="55"/>
+      <c r="L9" s="54"/>
     </row>
     <row r="10" ht="21.75" customHeight="1">
       <c r="A10" s="38"/>
@@ -9389,7 +9407,7 @@
       <c r="I10" s="40"/>
       <c r="J10" s="40"/>
       <c r="K10" s="40"/>
-      <c r="L10" s="55"/>
+      <c r="L10" s="54"/>
     </row>
     <row r="11" ht="21.75" customHeight="1">
       <c r="A11" s="38"/>
@@ -9403,7 +9421,7 @@
       <c r="I11" s="40"/>
       <c r="J11" s="40"/>
       <c r="K11" s="40"/>
-      <c r="L11" s="55"/>
+      <c r="L11" s="54"/>
     </row>
     <row r="12" ht="21.75" customHeight="1">
       <c r="A12" s="38"/>
@@ -9417,7 +9435,7 @@
       <c r="I12" s="40"/>
       <c r="J12" s="40"/>
       <c r="K12" s="40"/>
-      <c r="L12" s="55"/>
+      <c r="L12" s="54"/>
     </row>
     <row r="13" ht="21.75" customHeight="1">
       <c r="A13" s="38"/>
@@ -9431,7 +9449,7 @@
       <c r="I13" s="40"/>
       <c r="J13" s="40"/>
       <c r="K13" s="40"/>
-      <c r="L13" s="55"/>
+      <c r="L13" s="54"/>
     </row>
     <row r="14" ht="21.75" customHeight="1">
       <c r="A14" s="38"/>
@@ -9445,7 +9463,7 @@
       <c r="I14" s="40"/>
       <c r="J14" s="40"/>
       <c r="K14" s="40"/>
-      <c r="L14" s="55"/>
+      <c r="L14" s="54"/>
     </row>
     <row r="15" ht="21.75" customHeight="1">
       <c r="A15" s="38"/>
@@ -9459,7 +9477,7 @@
       <c r="I15" s="40"/>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
-      <c r="L15" s="55"/>
+      <c r="L15" s="54"/>
     </row>
     <row r="16" ht="21.75" customHeight="1">
       <c r="A16" s="38"/>
@@ -9473,7 +9491,7 @@
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
-      <c r="L16" s="55"/>
+      <c r="L16" s="54"/>
     </row>
     <row r="17" ht="21.75" customHeight="1">
       <c r="A17" s="38"/>
@@ -9487,7 +9505,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
-      <c r="L17" s="55"/>
+      <c r="L17" s="54"/>
     </row>
     <row r="18" ht="21.75" customHeight="1">
       <c r="A18" s="38"/>
@@ -9501,7 +9519,7 @@
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
       <c r="K18" s="40"/>
-      <c r="L18" s="55"/>
+      <c r="L18" s="54"/>
     </row>
     <row r="19" ht="21.75" customHeight="1">
       <c r="A19" s="38"/>
@@ -9515,7 +9533,7 @@
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
-      <c r="L19" s="55"/>
+      <c r="L19" s="54"/>
     </row>
     <row r="20" ht="21.75" customHeight="1">
       <c r="A20" s="38"/>
@@ -9529,7 +9547,7 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
       <c r="K20" s="40"/>
-      <c r="L20" s="55"/>
+      <c r="L20" s="54"/>
     </row>
     <row r="21" ht="21.75" customHeight="1">
       <c r="A21" s="38"/>
@@ -9543,7 +9561,7 @@
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
       <c r="K21" s="40"/>
-      <c r="L21" s="55"/>
+      <c r="L21" s="54"/>
     </row>
     <row r="22" ht="21.75" customHeight="1">
       <c r="A22" s="38"/>
@@ -9557,7 +9575,7 @@
       <c r="I22" s="40"/>
       <c r="J22" s="40"/>
       <c r="K22" s="40"/>
-      <c r="L22" s="55"/>
+      <c r="L22" s="54"/>
     </row>
     <row r="23" ht="21.75" customHeight="1">
       <c r="A23" s="38"/>
@@ -9571,7 +9589,7 @@
       <c r="I23" s="40"/>
       <c r="J23" s="40"/>
       <c r="K23" s="40"/>
-      <c r="L23" s="55"/>
+      <c r="L23" s="54"/>
     </row>
     <row r="24" ht="21.75" customHeight="1">
       <c r="A24" s="42"/>
@@ -9585,7 +9603,7 @@
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
-      <c r="L24" s="56"/>
+      <c r="L24" s="55"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>

</xml_diff>